<commit_message>
Sample File Has Been Set
</commit_message>
<xml_diff>
--- a/public/images/inventory Sample File.xlsx
+++ b/public/images/inventory Sample File.xlsx
@@ -1,20 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27528"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A631439D-1815-4A0D-93D7-ADC981D3307C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="550" windowWidth="15040" windowHeight="6740"/>
+    <workbookView xWindow="270" yWindow="550" windowWidth="15040" windowHeight="6740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INVENTORY_SAMPLE_BULK_INV_NOT_P" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>SIM</t>
   </si>
@@ -27,23 +44,11 @@
   <si>
     <t>IMEI</t>
   </si>
-  <si>
-    <t>Micro</t>
-  </si>
-  <si>
-    <t>767676TEST8798</t>
-  </si>
-  <si>
-    <t>268435492203335005</t>
-  </si>
-  <si>
-    <t>BOX no</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -83,13 +88,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -97,6 +100,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -297,51 +308,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.90625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="12.6328125" customWidth="1"/>
-    <col min="3" max="3" width="12.6328125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.6328125" style="4"/>
+    <col min="1" max="1" width="20.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="A2" s="4"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="4" spans="1:4" ht="15.75" customHeight="1"/>

</xml_diff>